<commit_message>
Fix bug same size in slips
</commit_message>
<xml_diff>
--- a/Database/packing_list_database.xlsx
+++ b/Database/packing_list_database.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="93">
   <si>
     <t>Ma hang</t>
   </si>
@@ -67,9 +67,6 @@
     <t>FA0293-4</t>
   </si>
   <si>
-    <t>F62469</t>
-  </si>
-  <si>
     <t>F62466</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>RA0293</t>
   </si>
   <si>
-    <t>R62469</t>
-  </si>
-  <si>
     <t>R62120</t>
   </si>
   <si>
@@ -95,6 +89,278 @@
   </si>
   <si>
     <t>RM62019</t>
+  </si>
+  <si>
+    <t>CMPT</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>MATERIAL FEE</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RA0308</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RM62003</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R76412</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RM62001</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R76411</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R61012</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>FM62003-3</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA0308</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA0307-1</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F76411</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F62470-3</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F61012-2</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>570*400*280mm</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F62470</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RA0300</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RM62014</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F09008-4</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>FM62014</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>FM62015</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RA0307</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RA0308</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F62469</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>M22013</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F62470</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>M11028</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>M12013</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RM62015</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R09008</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F64086</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA0299</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA0299-3</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RA0299</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R64086</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RA0300</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R64063</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F64063</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F62466-3</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R08012</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R08013</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F08012</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>FM62010</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F08013-3</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R682016</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R682017</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R682019</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F682017-4</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F682016-3</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R962470</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R682025</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R682026</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R682027</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R682028</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F962469</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F962470</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F962470-3</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F682025</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F682026-3</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>B631051</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>FM62018</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R682016</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R682019</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>F62120</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R62473</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>RM62009</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>R62469</t>
+    <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -104,7 +370,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +437,7 @@
     <font>
       <sz val="12"/>
       <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -195,6 +462,19 @@
       <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -6809,12 +7089,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -10653,19 +10945,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1">
@@ -10675,14 +10968,20 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1">
@@ -10692,14 +10991,20 @@
       <c r="B2" s="2">
         <v>56</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>4.6399999999999997</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>5.98</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3.42</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10709,17 +11014,21 @@
       <c r="B3" s="2">
         <v>72</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>4.74</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>6.08</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.58</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -10731,17 +11040,21 @@
       <c r="B4" s="2">
         <v>72</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>4.74</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>6.08</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.77</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -10753,17 +11066,21 @@
       <c r="B5" s="2">
         <v>64</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>5.74</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.5099999999999998</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -10775,17 +11092,21 @@
       <c r="B6" s="2">
         <v>360</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>7.06</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>8.1199999999999992</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.55</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -10797,17 +11118,21 @@
       <c r="B7" s="2">
         <v>360</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>10.36</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>11.42</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.84</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -10819,17 +11144,21 @@
       <c r="B8" s="2">
         <v>360</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>9.56</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>10.62</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.61</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -10841,17 +11170,21 @@
       <c r="B9" s="2">
         <v>360</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>6.24</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>7.3</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.82</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -10863,113 +11196,161 @@
       <c r="B10" s="2">
         <v>120</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>11.06</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>12.12</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.71</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <v>360</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.85</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>360</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+        <v>240</v>
+      </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.1100000000000001</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2">
         <v>360</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="C13" s="3">
+        <v>9.59</v>
+      </c>
+      <c r="D13" s="3">
+        <v>10.65</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.84</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
-        <v>240</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+        <v>360</v>
+      </c>
+      <c r="C14" s="3">
+        <v>7.99</v>
+      </c>
+      <c r="D14" s="3">
+        <v>9.42</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.62</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2">
-        <v>360</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C15" s="3">
+        <v>6.06</v>
+      </c>
+      <c r="D15" s="3">
+        <v>7.22</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2.44</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="B16" s="2">
-        <v>360</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C16" s="3">
+        <v>6.01</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7.04</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -10979,59 +11360,87 @@
         <v>22</v>
       </c>
       <c r="B17" s="2">
-        <v>48</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="C17" s="3">
+        <v>6.84</v>
+      </c>
+      <c r="D17" s="3">
+        <v>8.18</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.58</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>72</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+        <v>360</v>
+      </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="F18" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.85</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2">
-        <v>60</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C19" s="3">
+        <v>4.46</v>
+      </c>
+      <c r="D19" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2.0699999999999998</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2">
-        <v>360</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C20" s="3">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>6.34</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -11040,345 +11449,1358 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>360</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="D21" s="3">
+        <v>4.96</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3.48</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="2">
-        <v>360</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.78</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2">
-        <v>72</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="G23" s="2">
+        <v>4.08</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2">
-        <v>72</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.66</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="F25" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="G25" s="2">
+        <v>2.85</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="F26" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2.72</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="F27" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.69</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="2">
+        <v>360</v>
+      </c>
+      <c r="C28" s="3">
+        <v>7.78</v>
+      </c>
+      <c r="D28" s="3">
+        <v>8.84</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1.1299999999999999</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="2">
+        <v>360</v>
+      </c>
+      <c r="C29" s="3">
+        <v>7.78</v>
+      </c>
+      <c r="D29" s="3">
+        <v>8.84</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1.19</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="F30" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.98</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="2">
+        <v>360</v>
+      </c>
+      <c r="C31" s="3">
+        <v>7.78</v>
+      </c>
+      <c r="D31" s="3">
+        <v>8.84</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.85</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="A32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="2">
+        <v>360</v>
+      </c>
+      <c r="C32" s="3">
+        <v>7.78</v>
+      </c>
+      <c r="D32" s="3">
+        <v>8.84</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.76</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="2"/>
+      <c r="A33" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="F33" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1.42</v>
+      </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="2">
+        <v>48</v>
+      </c>
+      <c r="C34" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D34" s="3">
+        <v>6.26</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G34" s="2">
+        <v>3.48</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="2">
+        <v>72</v>
+      </c>
+      <c r="C35" s="3">
+        <v>4.72</v>
+      </c>
+      <c r="D35" s="3">
+        <v>5.88</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1.19</v>
+      </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1.19</v>
+      </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="A37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="2">
+        <v>360</v>
+      </c>
+      <c r="C37" s="3">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="D37" s="3">
+        <v>11.08</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G37" s="2">
+        <v>2.0699999999999998</v>
+      </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="A38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="2">
+        <v>360</v>
+      </c>
+      <c r="C38" s="3">
+        <v>10.02</v>
+      </c>
+      <c r="D38" s="3">
+        <v>11.08</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G38" s="2">
+        <v>1.19</v>
+      </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="2">
+        <v>48</v>
+      </c>
+      <c r="C39" s="3">
+        <v>3.83</v>
+      </c>
+      <c r="D39" s="3">
+        <v>5.18</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G39" s="2">
+        <v>3.76</v>
+      </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="A40" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="2">
+        <v>48</v>
+      </c>
+      <c r="C40" s="3">
+        <v>3.76</v>
+      </c>
+      <c r="D40" s="3">
+        <v>5.48</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G40" s="2">
+        <v>3.48</v>
+      </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+      <c r="A41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="2">
+        <v>360</v>
+      </c>
+      <c r="C41" s="3">
+        <v>10.44</v>
+      </c>
+      <c r="D41" s="3">
+        <v>11.74</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="A42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="2">
+        <v>240</v>
+      </c>
+      <c r="C42" s="3">
+        <v>9.74</v>
+      </c>
+      <c r="D42" s="3">
+        <v>10.9</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="G42" s="2">
+        <v>1.62</v>
+      </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="A43" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="2">
+        <v>360</v>
+      </c>
+      <c r="C43" s="3">
+        <v>10.88</v>
+      </c>
+      <c r="D43" s="3">
+        <v>12.18</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.75</v>
+      </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
+      <c r="A44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="2">
+        <v>120</v>
+      </c>
+      <c r="C44" s="3">
+        <v>8.56</v>
+      </c>
+      <c r="D44" s="3">
+        <v>10.32</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="G44" s="2">
+        <v>3.28</v>
+      </c>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="2">
+        <v>120</v>
+      </c>
+      <c r="C45" s="3">
+        <v>5.52</v>
+      </c>
+      <c r="D45" s="3">
+        <v>7.28</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="G45" s="2">
+        <v>1.82</v>
+      </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
+      <c r="A46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="2">
+        <v>72</v>
+      </c>
+      <c r="C46" s="3">
+        <v>3.94</v>
+      </c>
+      <c r="D46" s="3">
+        <v>5.92</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G46" s="2">
+        <v>1.7</v>
+      </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
+      <c r="A47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="2">
+        <v>48</v>
+      </c>
+      <c r="C47" s="3">
+        <v>3.76</v>
+      </c>
+      <c r="D47" s="3">
+        <v>5.48</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G47" s="2">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="2">
+        <v>360</v>
+      </c>
+      <c r="C48" s="3">
+        <v>7.48</v>
+      </c>
+      <c r="D48" s="3">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="2">
+        <v>360</v>
+      </c>
+      <c r="C49" s="3">
+        <v>11.33</v>
+      </c>
+      <c r="D49" s="3">
+        <v>12.64</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="2">
+        <v>360</v>
+      </c>
+      <c r="C50" s="3">
+        <v>11.33</v>
+      </c>
+      <c r="D50" s="3">
+        <v>12.64</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G50" s="2">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="2">
+        <v>48</v>
+      </c>
+      <c r="C51" s="3">
+        <v>4.66</v>
+      </c>
+      <c r="D51" s="3">
+        <v>5.94</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G51" s="2">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="2">
+        <v>48</v>
+      </c>
+      <c r="C52" s="3">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="D52" s="3">
+        <v>5.28</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G52" s="2">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="2">
+        <v>48</v>
+      </c>
+      <c r="C53" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="D53" s="3">
+        <v>6.62</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G53" s="2">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="2">
+        <v>48</v>
+      </c>
+      <c r="C54" s="3">
+        <v>4.08</v>
+      </c>
+      <c r="D54" s="3">
+        <v>5.36</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G54" s="2">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="2">
+        <v>360</v>
+      </c>
+      <c r="C55" s="3">
+        <v>9.42</v>
+      </c>
+      <c r="D55" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" s="2">
+        <v>48</v>
+      </c>
+      <c r="C57" s="3">
+        <v>2.06</v>
+      </c>
+      <c r="D57" s="3">
+        <v>3.78</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G57" s="2">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="2">
+        <v>360</v>
+      </c>
+      <c r="C59" s="3">
+        <v>8.34</v>
+      </c>
+      <c r="D59" s="3">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G59" s="2">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G60" s="2">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" s="5">
+        <v>360</v>
+      </c>
+      <c r="C61" s="3">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="D61" s="3">
+        <v>11</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="G61" s="2">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" s="5">
+        <v>72</v>
+      </c>
+      <c r="C62" s="3">
+        <v>5.88</v>
+      </c>
+      <c r="D62" s="3">
+        <v>7.04</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" s="5">
+        <v>72</v>
+      </c>
+      <c r="C63" s="3">
+        <v>5.48</v>
+      </c>
+      <c r="D63" s="3">
+        <v>6.64</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63" s="2">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64" s="5">
+        <v>72</v>
+      </c>
+      <c r="C64" s="3">
+        <v>4.79</v>
+      </c>
+      <c r="D64" s="3">
+        <v>5.95</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" s="5">
+        <v>360</v>
+      </c>
+      <c r="C65" s="3">
+        <v>11.34</v>
+      </c>
+      <c r="D65" s="3">
+        <v>12.54</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F65" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" s="5">
+        <v>360</v>
+      </c>
+      <c r="C66" s="3">
+        <v>8.42</v>
+      </c>
+      <c r="D66" s="3">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="5">
+        <v>72</v>
+      </c>
+      <c r="C67" s="3">
+        <v>4.74</v>
+      </c>
+      <c r="D67" s="3">
+        <v>6.08</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68" s="5">
+        <v>72</v>
+      </c>
+      <c r="C68" s="3">
+        <v>6.53</v>
+      </c>
+      <c r="D68" s="3">
+        <v>7.84</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="5">
+        <v>72</v>
+      </c>
+      <c r="C69" s="3">
+        <v>6.06</v>
+      </c>
+      <c r="D69" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" s="5">
+        <v>72</v>
+      </c>
+      <c r="C70" s="3">
+        <v>6.06</v>
+      </c>
+      <c r="D70" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" s="5">
+        <v>72</v>
+      </c>
+      <c r="C71" s="3">
+        <v>6.06</v>
+      </c>
+      <c r="D71" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="5">
+        <v>72</v>
+      </c>
+      <c r="C72" s="3">
+        <v>6.06</v>
+      </c>
+      <c r="D72" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" s="5">
+        <v>360</v>
+      </c>
+      <c r="C73" s="3">
+        <v>9.92</v>
+      </c>
+      <c r="D73" s="3">
+        <v>10.98</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="5">
+        <v>360</v>
+      </c>
+      <c r="C74" s="3">
+        <v>9.92</v>
+      </c>
+      <c r="D74" s="3">
+        <v>10.98</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" s="5">
+        <v>360</v>
+      </c>
+      <c r="C75" s="3">
+        <v>9.92</v>
+      </c>
+      <c r="D75" s="3">
+        <v>10.98</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" s="5">
+        <v>360</v>
+      </c>
+      <c r="C76" s="3">
+        <v>9</v>
+      </c>
+      <c r="D76" s="3">
+        <v>10.06</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" s="5">
+        <v>360</v>
+      </c>
+      <c r="C77" s="3">
+        <v>9</v>
+      </c>
+      <c r="D77" s="3">
+        <v>10.06</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" s="5">
+        <v>360</v>
+      </c>
+      <c r="C78" s="3">
+        <v>6.44</v>
+      </c>
+      <c r="D78" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79" s="5">
+        <v>360</v>
+      </c>
+      <c r="C79" s="3">
+        <v>13.44</v>
+      </c>
+      <c r="D79" s="3">
+        <v>14.9</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" s="5">
+        <v>360</v>
+      </c>
+      <c r="C80" s="3">
+        <v>10.74</v>
+      </c>
+      <c r="D80" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" s="5">
+        <v>360</v>
+      </c>
+      <c r="C81" s="3">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="D81" s="3">
+        <v>11.18</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F81">
+        <v>0.83</v>
+      </c>
+      <c r="G81">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B82" s="5">
+        <v>72</v>
+      </c>
+      <c r="C82" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="D82" s="3">
+        <v>7.01</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F82">
+        <v>1.54</v>
+      </c>
+      <c r="G82">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" s="5">
+        <v>72</v>
+      </c>
+      <c r="C83" s="3">
+        <v>5.54</v>
+      </c>
+      <c r="D83" s="3">
+        <v>7</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="2">
+        <v>72</v>
+      </c>
+      <c r="C84" s="3">
+        <v>5.88</v>
+      </c>
+      <c r="D84" s="3">
+        <v>7.04</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F84">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="2">
+        <v>72</v>
+      </c>
+      <c r="C85" s="3">
+        <v>4.79</v>
+      </c>
+      <c r="D85" s="3">
+        <v>5.95</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F85">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="B86" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>